<commit_message>
Correções de daods para puxar o saldo anterior e primeira tentativa de baixar o resultado para o DRE
</commit_message>
<xml_diff>
--- a/static/modelos/modelo_balancete.xlsx
+++ b/static/modelos/modelo_balancete.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5B519E43-4566-4382-8A56-F40BA29A67F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A858FAED-7302-4947-9967-4601D6B5C30A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8F6C426B-C597-4145-8FF2-1C80A6962E0B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
   <si>
     <t>CONTA</t>
   </si>
@@ -128,9 +128,6 @@
     <t>8.1.9.99.00.001-3</t>
   </si>
   <si>
-    <t>SALDOATUAL</t>
-  </si>
-  <si>
     <t>1.0.0.00.00-7</t>
   </si>
   <si>
@@ -345,15 +342,20 @@
   </si>
   <si>
     <t>9.0.9.17.15.001-5</t>
+  </si>
+  <si>
+    <t>SALDO ATUAL</t>
+  </si>
+  <si>
+    <t>SALDO ANTERIOR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -364,6 +366,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -388,17 +391,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Moeda" xfId="1" builtinId="4"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -731,831 +732,1136 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C51365E4-7133-4DB6-BCD0-78C66EAAEED5}">
-  <dimension ref="A1:B102"/>
+  <dimension ref="A1:C102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" s="1">
+        <v>29518224.949999999</v>
+      </c>
+      <c r="C2" s="1">
+        <v>32991133.09</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="2">
-        <v>32991133.09</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" s="1">
+        <v>7878627.3600000003</v>
+      </c>
+      <c r="C3" s="1">
+        <v>11354527.76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B4" s="1">
+        <v>7878627.3600000003</v>
+      </c>
+      <c r="C4" s="1">
         <v>11354527.76</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B5" s="1">
+        <v>7878627.3600000003</v>
+      </c>
+      <c r="C5" s="1">
         <v>11354527.76</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" s="2">
-        <v>11354527.76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
+        <v>7878627.3600000003</v>
+      </c>
+      <c r="C6" s="1">
         <v>11354527.76</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="1">
+        <v>21176210.390000001</v>
+      </c>
+      <c r="C12" s="1">
+        <v>20949086.449999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="2">
-        <v>20949086.449999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B13" s="1">
+        <v>41753455.869999997</v>
+      </c>
+      <c r="C13" s="1">
+        <v>40964565.350000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B14" s="1">
+        <v>41753455.869999997</v>
+      </c>
+      <c r="C14" s="1">
         <v>40964565.350000001</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="2">
-        <v>40964565.350000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
+        <v>35082690.75</v>
+      </c>
+      <c r="C15" s="1">
         <v>34339256.530000001</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
+        <v>6670765.1200000001</v>
+      </c>
+      <c r="C16" s="1">
         <v>6625308.8200000003</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="1">
+        <v>-20577245.48</v>
+      </c>
+      <c r="C17" s="1">
+        <v>-20015478.899999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B18" s="1">
+        <v>-20577245.48</v>
+      </c>
+      <c r="C18" s="1">
         <v>-20015478.899999999</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="2">
-        <v>-20015478.899999999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="1">
+        <v>-20577245.48</v>
+      </c>
+      <c r="C19" s="1">
         <v>-20015478.899999999</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="1">
+        <v>461777.31</v>
+      </c>
+      <c r="C20" s="1">
+        <v>687518.88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B21" s="1">
+        <v>461777.31</v>
+      </c>
+      <c r="C21" s="1">
         <v>687518.88</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B22" s="1">
+        <v>461777.31</v>
+      </c>
+      <c r="C22" s="1">
         <v>687518.88</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" s="2">
-        <v>687518.88</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="1">
+        <v>461777.31</v>
+      </c>
+      <c r="C23" s="1">
         <v>687518.88</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1609.89</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="B25" s="1">
+        <v>1609.89</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>49</v>
-      </c>
-      <c r="B26" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="1">
+        <v>1609.89</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="1">
+        <v>1609.89</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="1">
+        <v>46783.42</v>
+      </c>
+      <c r="C28" s="1">
+        <v>46783.42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B29" s="1">
         <v>46783.42</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="C29" s="1">
+        <v>46783.42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>51</v>
       </c>
-      <c r="B29" s="2">
-        <v>46783.42</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="B30" s="1">
+        <v>23391.71</v>
+      </c>
+      <c r="C30" s="1">
+        <v>23391.71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>52</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B31" s="1">
         <v>23391.71</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="C31" s="1">
+        <v>23391.71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>53</v>
       </c>
-      <c r="B31" s="2">
-        <v>23391.71</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="B32" s="1">
+        <v>36539.279999999999</v>
+      </c>
+      <c r="C32" s="1">
+        <v>2591243.66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>54</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B33" s="1">
+        <v>36539.279999999999</v>
+      </c>
+      <c r="C33" s="1">
         <v>2591243.66</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>55</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B34" s="1">
+        <v>0</v>
+      </c>
+      <c r="C34" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" s="1">
+        <v>0</v>
+      </c>
+      <c r="C35" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>57</v>
+      </c>
+      <c r="B36" s="1">
+        <v>0</v>
+      </c>
+      <c r="C36" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>58</v>
+      </c>
+      <c r="B37" s="1">
+        <v>0</v>
+      </c>
+      <c r="C37" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" s="1">
+        <v>0</v>
+      </c>
+      <c r="C38" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>60</v>
+      </c>
+      <c r="B39" s="1">
+        <v>36539.279999999999</v>
+      </c>
+      <c r="C39" s="1">
         <v>2591243.66</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>56</v>
-      </c>
-      <c r="B34" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>57</v>
-      </c>
-      <c r="B35" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>58</v>
-      </c>
-      <c r="B36" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>59</v>
-      </c>
-      <c r="B37" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>60</v>
-      </c>
-      <c r="B38" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>61</v>
       </c>
-      <c r="B39" s="2">
-        <v>2591243.66</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="B40" s="1">
+        <v>0</v>
+      </c>
+      <c r="C40" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>62</v>
       </c>
-      <c r="B40" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="B41" s="1">
+        <v>0</v>
+      </c>
+      <c r="C41" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>63</v>
       </c>
-      <c r="B41" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="B42" s="1">
+        <v>0</v>
+      </c>
+      <c r="C42" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>64</v>
       </c>
-      <c r="B42" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>65</v>
-      </c>
-      <c r="B43" s="2">
+      <c r="B43" s="1">
+        <v>36539.279999999999</v>
+      </c>
+      <c r="C43" s="1">
         <v>36635.72</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>8</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B44" s="1">
+        <v>18221.45</v>
+      </c>
+      <c r="C44" s="1">
         <v>18317.86</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>9</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B45" s="1">
+        <v>18317.830000000002</v>
+      </c>
+      <c r="C45" s="1">
         <v>18317.86</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>66</v>
-      </c>
-      <c r="B46" s="2">
+        <v>65</v>
+      </c>
+      <c r="B46" s="1">
+        <v>0</v>
+      </c>
+      <c r="C46" s="1">
         <v>2554607.94</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>10</v>
       </c>
-      <c r="B47" s="2">
+      <c r="B47" s="1">
+        <v>0</v>
+      </c>
+      <c r="C47" s="1">
         <v>2554607.94</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>66</v>
+      </c>
+      <c r="B48" s="1">
+        <v>43593981.299999997</v>
+      </c>
+      <c r="C48" s="1">
+        <v>43587981.299999997</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>67</v>
       </c>
-      <c r="B48" s="2">
+      <c r="B49" s="1">
+        <v>43593981.299999997</v>
+      </c>
+      <c r="C49" s="1">
         <v>43587981.299999997</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>68</v>
       </c>
-      <c r="B49" s="2">
-        <v>43587981.299999997</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="B50" s="1">
+        <v>25426146.390000001</v>
+      </c>
+      <c r="C50" s="1">
+        <v>25420146.390000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>69</v>
       </c>
-      <c r="B50" s="2">
-        <v>25420146.390000001</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="B51" s="1">
+        <v>25475867.02</v>
+      </c>
+      <c r="C51" s="1">
+        <v>25472058.109999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>70</v>
       </c>
-      <c r="B51" s="2">
+      <c r="B52" s="1">
+        <v>25475867.02</v>
+      </c>
+      <c r="C52" s="1">
         <v>25472058.109999999</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>71</v>
-      </c>
-      <c r="B52" s="2">
-        <v>25472058.109999999</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>11</v>
       </c>
-      <c r="B53" s="2">
+      <c r="B53" s="1">
+        <v>25475867.02</v>
+      </c>
+      <c r="C53" s="1">
         <v>25472058.109999999</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>72</v>
-      </c>
-      <c r="B54" s="2">
+        <v>71</v>
+      </c>
+      <c r="B54" s="1">
+        <v>-49720.63</v>
+      </c>
+      <c r="C54" s="1">
         <v>-51911.72</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>12</v>
       </c>
-      <c r="B55" s="2">
+      <c r="B55" s="1">
+        <v>-49720.63</v>
+      </c>
+      <c r="C55" s="1">
         <v>-51911.72</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>72</v>
+      </c>
+      <c r="B56" s="1">
+        <v>18167834.91</v>
+      </c>
+      <c r="C56" s="1">
+        <v>18167834.91</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>73</v>
       </c>
-      <c r="B56" s="2">
+      <c r="B57" s="1">
         <v>18167834.91</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>74</v>
-      </c>
-      <c r="B57" s="2">
+      <c r="C57" s="1">
         <v>18167834.91</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>13</v>
       </c>
-      <c r="B58" s="2">
+      <c r="B58" s="1">
         <v>10038600.98</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C58" s="1">
+        <v>10038600.98</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>14</v>
       </c>
-      <c r="B59" s="2">
+      <c r="B59" s="1">
         <v>8129233.9299999997</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C59" s="1">
+        <v>8129233.9299999997</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>74</v>
+      </c>
+      <c r="B60" s="1">
+        <v>93127365.930000007</v>
+      </c>
+      <c r="C60" s="1">
+        <v>94873225.549999997</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>75</v>
       </c>
-      <c r="B60" s="2">
+      <c r="B61" s="1">
+        <v>93127365.930000007</v>
+      </c>
+      <c r="C61" s="1">
         <v>94873225.549999997</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>76</v>
       </c>
-      <c r="B61" s="2">
-        <v>94873225.549999997</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+      <c r="B62" s="1">
+        <v>92629762.230000004</v>
+      </c>
+      <c r="C62" s="1">
+        <v>94303398.400000006</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>77</v>
       </c>
-      <c r="B62" s="2">
+      <c r="B63" s="1">
+        <v>92629762.230000004</v>
+      </c>
+      <c r="C63" s="1">
         <v>94303398.400000006</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>78</v>
-      </c>
-      <c r="B63" s="2">
-        <v>94303398.400000006</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>15</v>
       </c>
-      <c r="B64" s="2">
+      <c r="B64" s="1">
+        <v>79948122.75</v>
+      </c>
+      <c r="C64" s="1">
         <v>81046021.150000006</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>16</v>
       </c>
-      <c r="B65" s="2">
+      <c r="B65" s="1">
+        <v>12681639.48</v>
+      </c>
+      <c r="C65" s="1">
         <v>13257377.25</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>78</v>
+      </c>
+      <c r="B66" s="1">
+        <v>267448.59000000003</v>
+      </c>
+      <c r="C66" s="1">
+        <v>326362.73</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>79</v>
       </c>
-      <c r="B66" s="2">
+      <c r="B67" s="1">
+        <v>267448.59000000003</v>
+      </c>
+      <c r="C67" s="1">
         <v>326362.73</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>80</v>
       </c>
-      <c r="B67" s="2">
+      <c r="B68" s="1">
+        <v>267448.59000000003</v>
+      </c>
+      <c r="C68" s="1">
         <v>326362.73</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>81</v>
-      </c>
-      <c r="B68" s="2">
-        <v>326362.73</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>17</v>
       </c>
-      <c r="B69" s="2">
+      <c r="B69" s="1">
+        <v>267448.59000000003</v>
+      </c>
+      <c r="C69" s="1">
         <v>326362.73</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>81</v>
+      </c>
+      <c r="B70" s="1">
+        <v>230155.11</v>
+      </c>
+      <c r="C70" s="1">
+        <v>243464.42</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>82</v>
       </c>
-      <c r="B70" s="2">
+      <c r="B71" s="1">
+        <v>230155.11</v>
+      </c>
+      <c r="C71" s="1">
         <v>243464.42</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>83</v>
-      </c>
-      <c r="B71" s="2">
-        <v>243464.42</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>18</v>
       </c>
-      <c r="B72" s="2">
+      <c r="B72" s="1">
+        <v>230155.11</v>
+      </c>
+      <c r="C72" s="1">
         <v>243464.42</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>83</v>
+      </c>
+      <c r="B73" s="1">
+        <v>-107239661.56</v>
+      </c>
+      <c r="C73" s="1">
+        <v>-108061317.42</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>84</v>
       </c>
-      <c r="B73" s="2">
+      <c r="B74" s="1">
+        <v>-107239661.56</v>
+      </c>
+      <c r="C74" s="1">
         <v>-108061317.42</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>85</v>
       </c>
-      <c r="B74" s="2">
-        <v>-108061317.42</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+      <c r="B75" s="1">
+        <v>-85611673.049999997</v>
+      </c>
+      <c r="C75" s="1">
+        <v>-86704111.019999996</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>86</v>
       </c>
-      <c r="B75" s="2">
+      <c r="B76" s="1">
+        <v>-85611673.049999997</v>
+      </c>
+      <c r="C76" s="1">
         <v>-86704111.019999996</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>87</v>
-      </c>
-      <c r="B76" s="2">
-        <v>-86704111.019999996</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>19</v>
       </c>
-      <c r="B77" s="2">
+      <c r="B77" s="1">
+        <v>-85611673.049999997</v>
+      </c>
+      <c r="C77" s="1">
         <v>-86704111.019999996</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>87</v>
+      </c>
+      <c r="B78" s="1">
+        <v>-2286254.52</v>
+      </c>
+      <c r="C78" s="1">
+        <v>-2577238.9900000002</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>88</v>
       </c>
-      <c r="B78" s="2">
-        <v>-2577238.9900000002</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>89</v>
-      </c>
-      <c r="B79" s="2">
+      <c r="B79" s="1">
+        <v>-1932</v>
+      </c>
+      <c r="C79" s="1">
         <v>-2192</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>20</v>
       </c>
-      <c r="B80" s="2">
+      <c r="B80" s="1">
+        <v>-1932</v>
+      </c>
+      <c r="C80" s="1">
         <v>-2192</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>90</v>
-      </c>
-      <c r="B81" s="2">
+        <v>89</v>
+      </c>
+      <c r="B81" s="1">
+        <v>-27906.19</v>
+      </c>
+      <c r="C81" s="1">
         <v>-30388.47</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>21</v>
       </c>
-      <c r="B82" s="2">
+      <c r="B82" s="1">
+        <v>-12756.91</v>
+      </c>
+      <c r="C82" s="1">
         <v>-13315.71</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>22</v>
       </c>
-      <c r="B83" s="2">
+      <c r="B83" s="1">
+        <v>-11039.25</v>
+      </c>
+      <c r="C83" s="1">
         <v>-12649.14</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>23</v>
       </c>
-      <c r="B84" s="2">
+      <c r="B84" s="1">
+        <v>-4110.03</v>
+      </c>
+      <c r="C84" s="1">
         <v>-4423.62</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>91</v>
-      </c>
-      <c r="B85" s="2">
+        <v>90</v>
+      </c>
+      <c r="B85" s="1">
+        <v>-1884450</v>
+      </c>
+      <c r="C85" s="1">
         <v>-2134450</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>24</v>
       </c>
-      <c r="B86" s="2">
+      <c r="B86" s="1">
         <v>-9450</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C86" s="1">
+        <v>-9450</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>25</v>
       </c>
-      <c r="B87" s="2">
+      <c r="B87" s="1">
+        <v>-1875000</v>
+      </c>
+      <c r="C87" s="1">
         <v>-2125000</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>92</v>
-      </c>
-      <c r="B88" s="2">
+        <v>91</v>
+      </c>
+      <c r="B88" s="1">
+        <v>-371966.33</v>
+      </c>
+      <c r="C88" s="1">
         <v>-408698.49</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>26</v>
       </c>
-      <c r="B89" s="2">
+      <c r="B89" s="1">
+        <v>-182446.47</v>
+      </c>
+      <c r="C89" s="1">
         <v>-200860.74</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>27</v>
       </c>
-      <c r="B90" s="2">
+      <c r="B90" s="1">
+        <v>-189519.86</v>
+      </c>
+      <c r="C90" s="1">
         <v>-207837.75</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>93</v>
-      </c>
-      <c r="B91" s="2">
+        <v>92</v>
+      </c>
+      <c r="B91" s="1">
+        <v>0</v>
+      </c>
+      <c r="C91" s="1">
         <v>-1510.03</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>28</v>
       </c>
-      <c r="B92" s="2">
+      <c r="B92" s="1">
+        <v>0</v>
+      </c>
+      <c r="C92" s="1">
         <v>-1510.03</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
+        <v>93</v>
+      </c>
+      <c r="B93" s="1">
+        <v>-19341733.989999998</v>
+      </c>
+      <c r="C93" s="1">
+        <v>-18779967.41</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>94</v>
       </c>
-      <c r="B93" s="2">
+      <c r="B94" s="1">
+        <v>-19341733.989999998</v>
+      </c>
+      <c r="C94" s="1">
         <v>-18779967.41</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>95</v>
-      </c>
-      <c r="B94" s="2">
-        <v>-18779967.41</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>29</v>
       </c>
-      <c r="B95" s="2">
+      <c r="B95" s="1">
+        <v>-19341733.989999998</v>
+      </c>
+      <c r="C95" s="1">
         <v>-18779967.41</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
+        <v>95</v>
+      </c>
+      <c r="B96" s="1">
+        <v>46783.42</v>
+      </c>
+      <c r="C96" s="1">
+        <v>46783.42</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
         <v>96</v>
       </c>
-      <c r="B96" s="2">
+      <c r="B97" s="1">
         <v>46783.42</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+      <c r="C97" s="1">
+        <v>46783.42</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>97</v>
       </c>
-      <c r="B97" s="2">
+      <c r="B98" s="1">
         <v>46783.42</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+      <c r="C98" s="1">
+        <v>46783.42</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>98</v>
       </c>
-      <c r="B98" s="2">
-        <v>46783.42</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+      <c r="B99" s="1">
+        <v>23391.71</v>
+      </c>
+      <c r="C99" s="1">
+        <v>23391.71</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>99</v>
       </c>
-      <c r="B99" s="2">
+      <c r="B100" s="1">
         <v>23391.71</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+      <c r="C100" s="1">
+        <v>23391.71</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>100</v>
       </c>
-      <c r="B100" s="2">
+      <c r="B101" s="1">
         <v>23391.71</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+      <c r="C101" s="1">
+        <v>23391.71</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>101</v>
       </c>
-      <c r="B101" s="2">
+      <c r="B102" s="1">
         <v>23391.71</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>102</v>
-      </c>
-      <c r="B102" s="2">
+      <c r="C102" s="1">
         <v>23391.71</v>
       </c>
     </row>

</xml_diff>